<commit_message>
add/modify test cases for zss-1320
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/unlocked.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/unlocked.xlsx
@@ -345,15 +345,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -363,8 +363,11 @@
       <c r="C1" s="1">
         <v>3</v>
       </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -375,7 +378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7</v>
       </c>
@@ -386,7 +389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>

</xml_diff>